<commit_message>
Añadido abstract y keywords a cada artículo.
</commit_message>
<xml_diff>
--- a/info/ISDM2024.xlsx
+++ b/info/ISDM2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">Tipo</t>
   </si>
   <si>
+    <t xml:space="preserve">Abstract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keywords</t>
+  </si>
+  <si>
     <t xml:space="preserve">Javier Cámara, Javier Troya, Lola Burgueño and Antonio Vallecillo</t>
   </si>
   <si>
@@ -43,24 +49,48 @@
     <t xml:space="preserve">relevante</t>
   </si>
   <si>
+    <t xml:space="preserve">Most experts agree that Large Language Models (LLMs), such as those used by Copilot and ChatGPT, are expected to revolutionize the way in which software is developed. Many papers are currently devoted to analyzing the potential advantages and limitations of these generative AI models for writing code. However, the analysis of the current state of LLMs with respect to software modeling has received little attention. In this paper, we investigate the current capabilities of ChatGPT to perform modeling tasks and to assist modelers, while also trying to identify its main shortcomings. Our findings show that, in contrast to code generation, the performance of the current version of ChatGPT for software modeling is limited, with various syntactic and semantic deficiencies, lack of consistency in responses, and scalability issues. We also outline our views on how we perceive the role that LLMs can play in the software modeling discipline in the short term, and how the modeling community can help to improve the current capabilities of ChatGPT and the coming LLMs for software modeling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Language Models, ChatGPT, Software models, Modeling languages, UML</t>
+  </si>
+  <si>
     <t xml:space="preserve">Meriem Ben Chaaben, Lola Burgueño and Houari Sahraoui</t>
   </si>
   <si>
     <t xml:space="preserve">Towards using Few-Shot Prompt Learning for Automating Model Completion</t>
   </si>
   <si>
+    <t xml:space="preserve">We propose a simple yet a novel approach to improve completion in domain modeling activities. Our approach exploits the power of large language models by using few-shot prompt learning without the need to train or fine-tune those models with large datasets that are scarce in this field. We implemented our approach and tested it on the completion of static and dynamic domain diagrams. Our initial evaluation shows that such an approach is effective and can be integrated in different ways during the modeling activities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language models, few-shot learning, prompt learning, domain modeling, model completion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Meysam Karimi, Shekoufeh Kolahdouz Rahimi and Javier Troya</t>
   </si>
   <si>
     <t xml:space="preserve">Ant-colony optimization for automating test model generation in model transformation testing (Summary)</t>
   </si>
   <si>
+    <t xml:space="preserve">In model transformation (MT) testing, test data generation is of key importance. However, test suites are not available out of the box, and existing approaches to generate them require to provide not only the metamodel to which the models must conform, but some other domain-specific artifacts. For instance, an MT developer aiming to perform an incremental implementation of an MT may need to count on a quality test suite from the very beginning, even before all MT requirements are clear, only having the metamodels as input. We propose a black-box approach for the generation of test models where only the input metamodel of the MT is available. We propose an Ant-Colony Optimization algorithm for the search of test models satisfying the objectives of maximizing internal diversity and maximizing external diversity. We provide a tool prototype that implements this approach and generates the models in the well-established XMI interchange format. A comparison study with state-of-the-art frameworks shows that models are generated in reasonable times with low memory consumption. We empirically demonstrate the adequacy of our approach to generate effective test models, obtaining an overall mutation score above 80% from an evaluation with more than 5000 MT mutants.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model-Driven Engineering, Model Transformation Testing, Automated Model Generation, Ant Colony Optimization</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cesar Gonzalez Mora, Cristina Barros, Irene Garrigos, Jose Zubcoff, Elena Lloret and Jose-Norberto Mazon</t>
   </si>
   <si>
     <t xml:space="preserve">Improving Open Data Web API Documentation through Interactivity and Natural Language Generation</t>
   </si>
   <si>
+    <t xml:space="preserve">Widely adoption of Information Technologies has resulted in the continuous growing of open data available on the Web. However, the lack of suitable mechanisms to understand open data sources hampers its reusability. One way to overcome this limitation is by means of Web Application Programming Interfaces (APIs) with proper documentation, nowadays being the existing very rudimentary, hard to follow, and sometimes incomplete or even inaccurate in most cases. In order to improve the documentation of Web APIs that access open data, this paper proposes a novel approach to automatically generate interactive Web API documentation, both machine and user readable. This process starts by analysing the documentation of an API to obtain important information, automatically constructing Natural Language descriptions of the main Web API concepts by applying Natural Language Processing (NLP), and specifically, language generation techniques. Then, the documentation is made interactive by making it available as a Web interface, offering easy access to open data provided by Web APIs. Therefore, the use and comprehension of the Web APIs is facilitated, thus promoting the reusability of open data. The feasibility of our approach is presented through a case study and an experiment with users, both showing the benefits of our approach.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web API, OpenAPI documentation, Natural Language Processing, Natural Language Generation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pedro Juan Molina Moreno and Javier Centeno Vega</t>
   </si>
   <si>
@@ -70,12 +100,24 @@
     <t xml:space="preserve">corto</t>
   </si>
   <si>
+    <t xml:space="preserve">Traditional Container Orchestration tools like Docker Compose and Kubernetes are command-line based and require experience with command line interfaces, and dealing with many configuration files written in YAML. The work presented: Orca is a graphical editor embracing the Nocode approach to provide a very simple and intuitive user interface experience to non-developers to be able to design, document, explore, and deploy non-trivial configurations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDE, DSL, nocode, containers, graphical editors, Docker, Artificial Intelligence</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rubén Salado-Cid, Antonio Vallecillo, Kamran Munir and José Raúl Romero</t>
   </si>
   <si>
     <t xml:space="preserve">SWEL: A Domain-Specific Language for Modeling Data-Intensive Workflows</t>
   </si>
   <si>
+    <t xml:space="preserve">Data-intensive applications aim at discovering valuable knowledge from large amounts of data coming from real-world sources. Typically, workflow languages are used to specify these applications, and their associated engines enable the execution of the specifications. However, as these applications become commonplace, new challenges arise. Existing workflow languages are normally platform-specific, which severely hinders their interoperability with other languages and execution engines. This also limits their reusability outside the platforms for which they were originally defined. Following the Design Science Research methodology, the paper presents SWEL (Scientific Workflow Execution Language). SWEL is a domain-specific modeling language for the specification of data-intensive workflows that follow the model-driven engineering principles, covering the high-level definition of tasks, information sources, platform requirements, and mappings to the target technologies. SWEL is platform-independent, enables collaboration among data scientists across multiple domains and facilitates interoperability. The evaluation results show that SWEL is suitable enough to represent the concepts and mechanisms of commonly used data-intensive workflows. Moreover, SWEL facilitates the development of related technologies such as editors, tools for exchanging knowledge assets between workflow management systems, and tools for collaborative workflow development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model-driven engineering, Domain-specific modeling, Conceptual modeling, Data-intensive applications, Data-driven workflows, Data science</t>
+  </si>
+  <si>
     <t xml:space="preserve">Guillermo Fuentes, Francisco Ruiz and Angelica Caro</t>
   </si>
   <si>
@@ -85,6 +127,12 @@
     <t xml:space="preserve">herramienta</t>
   </si>
   <si>
+    <t xml:space="preserve">Un punto de vista contiene un conjunto de acuerdos para construir y utilizar una vista arquitectural. Esto con el objetivo de centrarse en las preocupaciones de cierto interesado o grupo de interés. De esta forma, quien modela lo hace centrándose en el punto de vista y solo pondrá atención en lo que le preocupa. Archi es una herramienta gratuita y de código abierto, ampliamente utilizada para el modelado de descripciones de arquitectura empresarial con la notación ArchiMate. Esta herramienta permite utilizar puntos de vista pero carece de la capacidad de incorporar nuevos, lo cual restringe su adaptabilidad y flexibilidad. Nuestro trabajo presenta una mejora en Archi, permitiendo la importación de nuevos puntos de vista definidos por el usuario a través de un archivo con una estructura simple, aumentando así su alineamiento con las necesidades específicas de las organizaciones. Además, esta mejora promueve el intercambio de estas configuraciones a través de los archivos que se crean, mejorando el modelado colaborativo y adaptable en diversos proyectos de arquitectura empresarial.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arquitectura Empresarial, Archi, ArchiMate, Puntos de Vista</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abel Gómez, Iván Alfonso, Silvia Doñate, Jordi Cabot and Robert Clarisó</t>
   </si>
   <si>
@@ -94,10 +142,10 @@
     <t xml:space="preserve">completo</t>
   </si>
   <si>
-    <t xml:space="preserve">Rosendo Moreno Rodríguez and Suleiny Rodríguez Aguila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uso del ChatGPT para análisis de requisitos en módulo CIM-PIM</t>
+    <t xml:space="preserve">Wastewater treatment plants (WWTPs) are critical infrastructures that employ cyber-physical systems (CPSs) and Internet of Things technology to manage and treat water. These systems gather data from various components such as sensors and monitors. However, the distributed nature of these systems introduces significant security concerns. To address these concerns, role-based access control (RBAC) has emerged as a fundamental security mechanism to govern access and authorization within these distributed CPS environments. This paper presents an innovative approach that leverages model-driven engineering (MDE) to implement RBAC in the design and operation of WWTPs. By integrating RBAC specifications seamlessly within the CPS model, this approach ensures a coherent security framework throughout the system's lifecycle. The use of MDE enables the generation of code and the creation of role-based custom visualizations, improving user experience and strengthening data security. We highlight the potential of these modeling techniques using a real-world scenario from TRANSACT, a KDT Joint Undertaking aiming to provide a framework to transform standalone safety-critical CPSs into safe and secure distributed solutions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model-driven engineering (MDE), Role-based access control (RBAC), Wastewater treatment plant (WWTP), Code generation</t>
   </si>
   <si>
     <t xml:space="preserve">José Ángel Barriga Corchero, Pedro José Clemente Martín, Miguel Ángel Pérez Toledano, Elena Jurado Málaga and Juan María Hernández Núñez</t>
@@ -106,16 +154,34 @@
     <t xml:space="preserve">Design, code generation and simulation of IoT environments with mobility devices by using model-driven development: SimulateIoT-Mobile</t>
   </si>
   <si>
+    <t xml:space="preserve">The Internet of Things (IoT) is rapidly spreading across multiple sectors, such as the industry in general terms, which is well-known as the Industrial IoT (IIoT). However, it faces challenges, as in the case of device mobility management. Device mobility can cause problems such as packet loss, latency, and security risks, and is compounded by the lack of standardized mobility management in key IoT protocols such as MQTT or CoAP. To address these complexities, this paper presents a Domain Specific Language (DSL) based on SimulateIoT to design, validate, generate, and deploy IoT systems simulations focused on mobility management within the context of the MQTT protocol. The DSL facilitates the integration of components such as mobile sensors and actuators, stationary fog and cloud nodes, together with the components related to the mobility-supporting architecture. Finally, the effectiveness of this approach is demonstrated through two case studies: animal tracking and Personal Mobility Devices (PMD) in the context of smart cities, showing the practical deployment and functionality of the developed IoT solutions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IIoT systems, IoT simulation, IoT mobility, Model-driven development, Model-to-text transformation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cristian Gómez Macías, Juan Manuel Vara, Francisco Javier Perez Blanco, David Granada and Carlos Villarrubia</t>
   </si>
   <si>
     <t xml:space="preserve">Soportando la producción de contratos inteligentes a partir de modelos de negocio</t>
   </si>
   <si>
+    <t xml:space="preserve">Este trabajo presenta el desarrollo de SmaCQA, un DSL textual que permite recoger información de bajo nivel sobre los intercambios de valor representados en modelos de valor expresados con la notación e{$^3$}value ya que, por su naturaleza, los modelos de valor no permiten recoger este tipo de información. La idea subyacente es utilizar esta información complementaria para facilitar la generación de contratos inteligentes a partir de modelos de valor. Para ilustrar la utilidad de la propuesta, el trabajo documenta un caso de estudio del mercado de la energía. Los resultados demuestran que la solución tecnológica desarrollada posibilita la generación de contratos inteligentes mucho más completos y complejos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smart Contracts, Model Driven Engineering, e3value, Business Modeling</t>
+  </si>
+  <si>
     <t xml:space="preserve">Damien Foures, Mathieu Acher, Olivier Barais, Benoit Combemale, Jean-Marc Jézéquel and Jörg Kienzle</t>
   </si>
   <si>
     <t xml:space="preserve">Experience in Specializing a Generic Realization Language for SPL Engineering at Airbus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In software product line (SPL) engineering, feature models are the de facto standard for modeling variability. A user can derive products out of a base model by selecting features of interest. Doing it automatically, however, requires a realization model, which is a de- scription of how a base model should be modified when a given feature is selected/unselected. A realization model then necessarily depends on the base metamodel, asking for ad hoc solutions that have flourished in recent years. In this paper, we propose Greal, a generic solution to this problem in the form of (1) a generic declarative realization language that can be automatically composed with one or more base metamodels to yield a domain-specific realization language and (2) a product derivation algorithm applying a realization model to a base model and a resolved model to yield a derived product. We describe how, on top of Greal, we specialized a realization language to support both positive and neg- ative variability, fit the syntax and semantics of the targeted language (BPMN) and take into account modeling practices at Airbus. We report on lessons learned of applying this approach on Program Development Plans based on business process models and discuss open problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Variability, Feature Models, Realization Models, Positive, Negative Variability, BPMN</t>
   </si>
 </sst>
 </file>
@@ -216,28 +282,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -424,202 +498,261 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="60"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="B5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="6" t="n">
         <v>57</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>6</v>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="4" t="n">
         <v>81</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="6" t="n">
         <v>91</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
+      <c r="B9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>94</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
-        <v>121</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
+      <c r="A12" s="6" t="n">
         <v>124</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
+      <c r="B12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>